<commit_message>
updated metadata, added .tre
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrl17/Desktop/Lee &amp; Hawkes 2020 Phytobiomes J/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrl17/Repos/Lee_Hawkes_PhytobiomesJ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E2755C-F54B-1F49-944A-3F34B0C0B18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6687677-5AD3-6740-A3CC-88DF41CA91EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1220" windowWidth="20440" windowHeight="14780" xr2:uid="{8A037AAE-0760-2443-A877-CBA808F7300F}"/>
+    <workbookView xWindow="5620" yWindow="460" windowWidth="20440" windowHeight="14780" xr2:uid="{8A037AAE-0760-2443-A877-CBA808F7300F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
   <si>
     <t>Metadata</t>
   </si>
@@ -47,16 +47,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>People</t>
-  </si>
-  <si>
     <t>NC-DOE-FIELD</t>
   </si>
   <si>
     <t>Sept/Oct 2018</t>
-  </si>
-  <si>
-    <t>ML = Marissa Lee, NY = Nathaniel Yang, IM = Isaiah McBryde, JC = Jacalyn Czel</t>
   </si>
   <si>
     <t>Description</t>
@@ -389,6 +383,39 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <t>TAXtree.tre</t>
+  </si>
+  <si>
+    <t>Newick-formated taxonomy-based hierarchy that was generated using the perl script "taxonomy_to_tree.perl" from Tedersoo et al (2008) and the taxonomy matrix from this study</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Year Published</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Plant and soil drivers of whole-plant microbiomes: variation in switchgrass fungi from coastal to mountain sites</t>
+  </si>
+  <si>
+    <t>Phytobiomes J.</t>
+  </si>
+  <si>
+    <t>Lee &amp; Hawkes</t>
+  </si>
+  <si>
+    <t>In press</t>
   </si>
 </sst>
 </file>
@@ -471,7 +498,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -487,6 +514,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C175F55-0471-3C4D-BEDA-0233C5995B1C}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -836,707 +864,751 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1"/>
+      <c r="B4" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
+      <c r="C11" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2"/>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2"/>
+      <c r="B18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="C26" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2"/>
-      <c r="B15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="10" t="s">
+      <c r="C27" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="10" t="s">
+      <c r="D28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16">
+      <c r="B29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="10" t="s">
+      <c r="D29" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C30" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="16">
-      <c r="B26" s="10" t="s">
+      <c r="E30" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16">
+      <c r="B31" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="10" t="s">
+      <c r="C31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="16">
-      <c r="B28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="E32" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C55" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="12" t="s">
-        <v>112</v>
-      </c>
       <c r="E55" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>